<commit_message>
Add carrier commission report and db-fix scripts
</commit_message>
<xml_diff>
--- a/docs/design/Carrier Commission Report COPY.xlsx
+++ b/docs/design/Carrier Commission Report COPY.xlsx
@@ -1436,8 +1436,8 @@
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
-    <TaxCatchAll xmlns="080f2c63-9d64-43b2-8af4-58ced9ff227e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a8d7c63e-97b8-40d8-a53b-a3ea59517dfc">
+    <TaxCatchAll xmlns="47b13cbd-3c99-4ce2-9493-8a1853fbc45d" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="65b177fb-a871-4436-ae31-3f4cb87c55ec">
       <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
@@ -1454,10 +1454,10 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007C874A60EE6D774BAF5AC34E0D014A52" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="58b2df5a6f8c7e5cc56b7ba40a008344">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a8d7c63e-97b8-40d8-a53b-a3ea59517dfc" xmlns:ns3="080f2c63-9d64-43b2-8af4-58ced9ff227e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="102fef89b1def977514bd1c02a7492c1" ns2:_="" ns3:_="">
-    <xsd:import namespace="a8d7c63e-97b8-40d8-a53b-a3ea59517dfc"/>
-    <xsd:import namespace="080f2c63-9d64-43b2-8af4-58ced9ff227e"/>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000EEB047874376646B9FCEA443C7CBFC9" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="57f0f4bcad47b8fbfb4f6b48fcae712a">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="65b177fb-a871-4436-ae31-3f4cb87c55ec" xmlns:ns3="47b13cbd-3c99-4ce2-9493-8a1853fbc45d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4bf2a65b24669de7801e6f4159825012" ns2:_="" ns3:_="">
+    <xsd:import namespace="65b177fb-a871-4436-ae31-3f4cb87c55ec"/>
+    <xsd:import namespace="47b13cbd-3c99-4ce2-9493-8a1853fbc45d"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -1466,15 +1466,10 @@
               <xsd:all>
                 <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
                 <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
                 <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
@@ -1485,7 +1480,7 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="a8d7c63e-97b8-40d8-a53b-a3ea59517dfc" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="65b177fb-a871-4436-ae31-3f4cb87c55ec" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
@@ -1498,86 +1493,45 @@
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="12" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="11" nillable="true" ma:displayName="MediaServiceDateTaken" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="13" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="14" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceSearchProperties" ma:index="15" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="17" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="063228c5-36a5-43ca-9dd4-4f5cf61fc59d" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="ff5c36b0-bf2f-41bb-a840-c6ab7967656e" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
         </xsd:sequence>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="MediaServiceLocation" ma:index="19" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="20" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="21" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="22" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="080f2c63-9d64-43b2-8af4-58ced9ff227e" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="47b13cbd-3c99-4ce2-9493-8a1853fbc45d" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="10" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="11" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TaxCatchAll" ma:index="18" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{88733ea6-b52b-4c57-9e45-1ec264d796a6}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="080f2c63-9d64-43b2-8af4-58ced9ff227e">
+    <xsd:element name="TaxCatchAll" ma:index="14" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{6df507dd-b16c-4176-bae6-6febb1b9c5a2}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="47b13cbd-3c99-4ce2-9493-8a1853fbc45d">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:MultiChoiceLookup">
@@ -1708,20 +1662,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFAC9D76-87B4-4D4D-BE46-45DB2FADBB73}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a8d7c63e-97b8-40d8-a53b-a3ea59517dfc"/>
-    <ds:schemaRef ds:uri="080f2c63-9d64-43b2-8af4-58ced9ff227e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A4E981D-5C0C-4253-9732-4188D235C81D}"/>
 </file>
</xml_diff>